<commit_message>
Updated cleaned data for Raigarh in Maharashtra which had parsing issues.
</commit_message>
<xml_diff>
--- a/phase 2 release/districts extract/unique ph201d Indicators_cleaned.xlsx
+++ b/phase 2 release/districts extract/unique ph201d Indicators_cleaned.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\code\external\nfhs5_factsheets\phase 2 release\districts extract\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0DDF164-E1C8-4950-A3A9-6BFFE7835F95}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69436148-2006-4213-B549-B971AD1A36C8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="20" windowWidth="16100" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="158">
   <si>
     <t>Indicator</t>
   </si>
@@ -475,16 +475,25 @@
     <t>80. Women who have high risk waist-to-hip ratio (&gt; 0.85) (%)</t>
   </si>
   <si>
-    <t>93. Moderately or severely elevated blood pressure (Systolic &gt; 160mm of Hg and/or Diastolic &gt; 100mm of Hg) (%)</t>
-  </si>
-  <si>
-    <t>94. Elevated blood pressure (Systolic &gt; 140 mm of Hg and/or Diastolic &gt; 90 mm of Hg) or taking medicine to control blood pressure (%)</t>
-  </si>
-  <si>
-    <t>96. Moderately or severely elevated blood pressure (Systolic &gt; 160mm of Hg and/or Diastolic &gt; 100mm of Hg) (%)</t>
-  </si>
-  <si>
-    <t>97. Elevated blood pressure (Systolic &gt; 140 mm of Hg and/or Diastolic &gt; 90 mm of Hg) or taking medicine to control blood pressure (%)</t>
+    <t>20. Any method6 (%)</t>
+  </si>
+  <si>
+    <t>79. Women who are overweight or obese (BMI ≥25.0 kg/m2)21 (%)</t>
+  </si>
+  <si>
+    <t>80. Women who have high risk waist-to-hip ratio (≥0.85) (%)</t>
+  </si>
+  <si>
+    <t>93. Moderately or severely elevated blood pressure (Systolic ≥160mm of Hg and/or Diastolic ≥100mm of Hg) (%)</t>
+  </si>
+  <si>
+    <t>94. Elevated blood pressure (Systolic ≥140 mm of Hg and/or Diastolic ≥90 mm of Hg) or taking medicine to control blood pressure (%)</t>
+  </si>
+  <si>
+    <t>96. Moderately or severely elevated blood pressure (Systolic ≥160mm of Hg and/or Diastolic ≥100mm of Hg) (%)</t>
+  </si>
+  <si>
+    <t>97. Elevated blood pressure (Systolic ≥140 mm of Hg and/or Diastolic ≥90 mm of Hg) or taking medicine to control blood pressure (%)</t>
   </si>
 </sst>
 </file>
@@ -537,7 +546,17 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -882,10 +901,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C149"/>
+  <dimension ref="A1:C155"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" topLeftCell="A137" workbookViewId="0">
+      <selection activeCell="C148" sqref="C148"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2154,371 +2173,425 @@
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A116" t="s">
-        <v>115</v>
-      </c>
-      <c r="B116">
-        <v>700</v>
+        <v>152</v>
       </c>
       <c r="C116" t="s">
-        <v>115</v>
+        <v>149</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A117" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B117">
         <v>700</v>
       </c>
       <c r="C117" t="s">
-        <v>150</v>
+        <v>115</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A118" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B118">
         <v>700</v>
       </c>
       <c r="C118" t="s">
-        <v>117</v>
+        <v>150</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A119" t="s">
-        <v>118</v>
-      </c>
-      <c r="B119">
-        <v>700</v>
+        <v>153</v>
       </c>
       <c r="C119" t="s">
-        <v>118</v>
+        <v>150</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A120" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B120">
         <v>700</v>
       </c>
       <c r="C120" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A121" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B121">
         <v>700</v>
       </c>
       <c r="C121" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A122" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B122">
         <v>700</v>
       </c>
       <c r="C122" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A123" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B123">
         <v>700</v>
       </c>
       <c r="C123" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A124" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B124">
         <v>700</v>
       </c>
       <c r="C124" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A125" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B125">
         <v>700</v>
       </c>
       <c r="C125" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A126" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B126">
         <v>700</v>
       </c>
       <c r="C126" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A127" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B127">
         <v>700</v>
       </c>
       <c r="C127" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A128" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B128">
         <v>700</v>
       </c>
       <c r="C128" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A129" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B129">
         <v>700</v>
       </c>
       <c r="C129" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A130" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B130">
         <v>700</v>
       </c>
       <c r="C130" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A131" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B131">
         <v>700</v>
       </c>
       <c r="C131" t="s">
-        <v>151</v>
+        <v>128</v>
       </c>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A132" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B132">
-        <v>1</v>
+        <v>700</v>
       </c>
       <c r="C132" t="s">
-        <v>152</v>
+        <v>129</v>
       </c>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A133" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B133">
-        <v>699</v>
+        <v>700</v>
       </c>
       <c r="C133" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A134" t="s">
-        <v>133</v>
-      </c>
-      <c r="B134">
-        <v>700</v>
+        <v>154</v>
       </c>
       <c r="C134" t="s">
-        <v>133</v>
+        <v>154</v>
       </c>
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A135" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="B135">
-        <v>700</v>
+        <v>1</v>
       </c>
       <c r="C135" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A136" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="B136">
-        <v>1</v>
+        <v>699</v>
       </c>
       <c r="C136" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A137" t="s">
-        <v>136</v>
-      </c>
-      <c r="B137">
-        <v>699</v>
+        <v>155</v>
       </c>
       <c r="C137" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A138" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="B138">
-        <v>187</v>
+        <v>700</v>
       </c>
       <c r="C138" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A139" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="B139">
-        <v>513</v>
+        <v>700</v>
       </c>
       <c r="C139" t="s">
-        <v>138</v>
+        <v>156</v>
       </c>
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A140" t="s">
-        <v>139</v>
-      </c>
-      <c r="B140">
-        <v>187</v>
+        <v>156</v>
       </c>
       <c r="C140" t="s">
-        <v>140</v>
+        <v>156</v>
       </c>
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A141" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="B141">
-        <v>513</v>
+        <v>1</v>
       </c>
       <c r="C141" t="s">
-        <v>140</v>
+        <v>157</v>
       </c>
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A142" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="B142">
-        <v>2</v>
+        <v>699</v>
+      </c>
+      <c r="C142" t="s">
+        <v>157</v>
       </c>
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A143" t="s">
-        <v>142</v>
-      </c>
-      <c r="B143">
-        <v>698</v>
+        <v>157</v>
       </c>
       <c r="C143" t="s">
-        <v>142</v>
+        <v>157</v>
       </c>
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A144" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="B144">
-        <v>2</v>
+        <v>187</v>
       </c>
       <c r="C144" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A145" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="B145">
-        <v>1</v>
+        <v>513</v>
       </c>
       <c r="C145" t="s">
-        <v>64</v>
+        <v>137</v>
       </c>
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A146" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="B146">
-        <v>1</v>
+        <v>187</v>
       </c>
       <c r="C146" t="s">
-        <v>69</v>
+        <v>139</v>
       </c>
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A147" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="B147">
-        <v>1</v>
+        <v>513</v>
       </c>
       <c r="C147" t="s">
-        <v>99</v>
+        <v>139</v>
       </c>
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A148" t="s">
+        <v>141</v>
+      </c>
+      <c r="B148">
+        <v>2</v>
+      </c>
+      <c r="C148" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="149" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A149" t="s">
+        <v>142</v>
+      </c>
+      <c r="B149">
+        <v>698</v>
+      </c>
+      <c r="C149" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="150" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A150" t="s">
+        <v>143</v>
+      </c>
+      <c r="B150">
+        <v>2</v>
+      </c>
+      <c r="C150" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="151" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A151" t="s">
+        <v>144</v>
+      </c>
+      <c r="B151">
+        <v>1</v>
+      </c>
+      <c r="C151" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="152" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A152" t="s">
+        <v>145</v>
+      </c>
+      <c r="B152">
+        <v>1</v>
+      </c>
+      <c r="C152" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="153" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A153" t="s">
+        <v>146</v>
+      </c>
+      <c r="B153">
+        <v>1</v>
+      </c>
+      <c r="C153" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="154" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A154" t="s">
         <v>147</v>
       </c>
-      <c r="B148">
+      <c r="B154">
         <v>1</v>
       </c>
-      <c r="C148" t="s">
+      <c r="C154" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="149" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B149">
+    <row r="155" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B155">
         <v>7</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="C1:C1048576">
+    <cfRule type="duplicateValues" dxfId="1" priority="2"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A1:A1048576">
     <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>